<commit_message>
création d'un fichier excel contenant les liens vers les dossier ou fichier (demande de l'entreprise pour plus de flexibilité). Problème avec location.href . Modification de la page Admin pour modifier plus facilement l'interface (ajout suppretion de bouton)
</commit_message>
<xml_diff>
--- a/init/CheminsDossier.xlsx
+++ b/init/CheminsDossier.xlsx
@@ -34,43 +34,43 @@
     <t>chemin absolue</t>
   </si>
   <si>
+    <t>Dossier contenant les extractions OF</t>
+  </si>
+  <si>
+    <t>Dossier contenant les IPR-Valides</t>
+  </si>
+  <si>
+    <t>Dossier contenant les IPR-autorisee</t>
+  </si>
+  <si>
+    <t>chemin pour l'application</t>
+  </si>
+  <si>
+    <t>W</t>
+  </si>
+  <si>
+    <t>EOLE-SAP</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>Services</t>
+  </si>
+  <si>
+    <t>Lecteur</t>
+  </si>
+  <si>
+    <t>Nom réseau</t>
+  </si>
+  <si>
+    <t>S:\Methodes Production\0- IPR VALIDE</t>
+  </si>
+  <si>
+    <t>S:\Methodes Production\1- IPR AUTORISEES</t>
+  </si>
+  <si>
     <t>W:\CHARGE_SAP\Extraction_OF</t>
-  </si>
-  <si>
-    <t>Dossier contenant les extractions OF</t>
-  </si>
-  <si>
-    <t>Dossier contenant les IPR-Valides</t>
-  </si>
-  <si>
-    <t>Dossier contenant les IPR-autorisee</t>
-  </si>
-  <si>
-    <t>S:\Methodes Production\0- IPR VALIDE</t>
-  </si>
-  <si>
-    <t>S:\Methodes Production\1- IPR AUTORISEES</t>
-  </si>
-  <si>
-    <t>chemin pour l'application</t>
-  </si>
-  <si>
-    <t>W</t>
-  </si>
-  <si>
-    <t>EOLE-SAP</t>
-  </si>
-  <si>
-    <t>S</t>
-  </si>
-  <si>
-    <t>Services</t>
-  </si>
-  <si>
-    <t>Lecteur</t>
-  </si>
-  <si>
-    <t>Nom réseau</t>
   </si>
 </sst>
 </file>
@@ -526,14 +526,14 @@
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="34.42578125" customWidth="1"/>
     <col min="2" max="2" width="40.7109375" customWidth="1"/>
-    <col min="3" max="3" width="59.28515625" customWidth="1"/>
+    <col min="3" max="3" width="62.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -544,68 +544,68 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="C2" s="2" t="str">
-        <f>SUBSTITUTE(SUBSTITUTE(B2,"W:","\\val-fs01\EOLE-SAP"),"\","\\")</f>
-        <v>\\\\val-fs01\\EOLE-SAP\\CHARGE_SAP\\Extraction_OF</v>
+        <f>SUBSTITUTE(SUBSTITUTE(B2,"W:","\\val-fs01\EOLE-SAP"),"\","\")</f>
+        <v>\\val-fs01\EOLE-SAP\CHARGE_SAP\Extraction_OF</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C3" s="2" t="str">
-        <f>SUBSTITUTE(SUBSTITUTE(B3,"S:","\\val-fs01\Services"),"\","\\")</f>
-        <v>\\\\val-fs01\\Services\\Methodes Production\\0- IPR VALIDE</v>
+        <f>SUBSTITUTE(SUBSTITUTE(B3,"S:","\\val-fs01\Services"),"\","\")</f>
+        <v>\\val-fs01\Services\Methodes Production\0- IPR VALIDE</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="C4" s="2" t="str">
-        <f>SUBSTITUTE(SUBSTITUTE(B4,"S:","\\val-fs01\Services"),"\","\\")</f>
-        <v>\\\\val-fs01\\Services\\Methodes Production\\1- IPR AUTORISEES</v>
+        <f>SUBSTITUTE(SUBSTITUTE(B4,"S:","\\val-fs01\Services"),"\","\")</f>
+        <v>\\val-fs01\Services\Methodes Production\1- IPR AUTORISEES</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F6" s="3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F7" s="5" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F8" s="7" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="G8" s="8" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
modification de getLink plus général
</commit_message>
<xml_diff>
--- a/init/CheminsDossier.xlsx
+++ b/init/CheminsDossier.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>ce que l'on recherche</t>
   </si>
@@ -34,36 +34,9 @@
     <t>chemin absolue</t>
   </si>
   <si>
-    <t>Dossier contenant les extractions OF</t>
-  </si>
-  <si>
-    <t>Dossier contenant les IPR-Valides</t>
-  </si>
-  <si>
-    <t>Dossier contenant les IPR-autorisee</t>
-  </si>
-  <si>
     <t>chemin pour l'application</t>
   </si>
   <si>
-    <t>W</t>
-  </si>
-  <si>
-    <t>EOLE-SAP</t>
-  </si>
-  <si>
-    <t>S</t>
-  </si>
-  <si>
-    <t>Services</t>
-  </si>
-  <si>
-    <t>Lecteur</t>
-  </si>
-  <si>
-    <t>Nom réseau</t>
-  </si>
-  <si>
     <t>S:\Methodes Production\0- IPR VALIDE</t>
   </si>
   <si>
@@ -71,6 +44,21 @@
   </si>
   <si>
     <t>W:\CHARGE_SAP\Extraction_OF</t>
+  </si>
+  <si>
+    <t>S:\Methodes Production\IPR CARTE CMS\FICHE D'INSTRUCTION</t>
+  </si>
+  <si>
+    <t>Extraction OF</t>
+  </si>
+  <si>
+    <t>IPR Valide</t>
+  </si>
+  <si>
+    <t>IPR Autorisee</t>
+  </si>
+  <si>
+    <t>IPR Carte CMS</t>
   </si>
 </sst>
 </file>
@@ -102,7 +90,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -125,124 +113,24 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -523,17 +411,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="34.42578125" customWidth="1"/>
-    <col min="2" max="2" width="40.7109375" customWidth="1"/>
-    <col min="3" max="3" width="62.28515625" customWidth="1"/>
+    <col min="2" max="2" width="58.7109375" customWidth="1"/>
+    <col min="3" max="3" width="73.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -544,15 +432,15 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="C2" s="2" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(B2,"W:","\\val-fs01\EOLE-SAP"),"\","\")</f>
@@ -561,10 +449,10 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>3</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>12</v>
       </c>
       <c r="C3" s="2" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(B3,"S:","\\val-fs01\Services"),"\","\")</f>
@@ -573,40 +461,51 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>4</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>13</v>
       </c>
       <c r="C4" s="2" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(B4,"S:","\\val-fs01\Services"),"\","\")</f>
         <v>\\val-fs01\Services\Methodes Production\1- IPR AUTORISEES</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="2" t="str">
+        <f>SUBSTITUTE(SUBSTITUTE(B5,"S:","\\val-fs01\Services"),"\","\")</f>
+        <v>\\val-fs01\Services\Methodes Production\IPR CARTE CMS\FICHE D'INSTRUCTION</v>
+      </c>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+    </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F6" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>11</v>
-      </c>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F7" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="G7" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F8" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="G8" s="8" t="s">
-        <v>9</v>
-      </c>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
modification du fichier excel pour concorder avec arborescence linux
</commit_message>
<xml_diff>
--- a/init/CheminsDossier.xlsx
+++ b/init/CheminsDossier.xlsx
@@ -414,14 +414,14 @@
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="34.42578125" customWidth="1"/>
     <col min="2" max="2" width="58.7109375" customWidth="1"/>
-    <col min="3" max="3" width="73.140625" customWidth="1"/>
+    <col min="3" max="3" width="81.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -443,8 +443,8 @@
         <v>5</v>
       </c>
       <c r="C2" s="2" t="str">
-        <f>SUBSTITUTE(SUBSTITUTE(B2,"W:","\\val-fs01\EOLE-SAP"),"\","/")</f>
-        <v>//val-fs01/EOLE-SAP/CHARGE_SAP/Extraction_OF</v>
+        <f>SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B2,"W:","/media/val-fs01/EOLE-SAP"),"\","/")," ","\ ")</f>
+        <v>/media/val-fs01/EOLE-SAP/CHARGE_SAP/Extraction_OF</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -455,8 +455,8 @@
         <v>3</v>
       </c>
       <c r="C3" s="2" t="str">
-        <f>SUBSTITUTE(SUBSTITUTE(B3,"S:","\\val-fs01\Services"),"\","/")</f>
-        <v>//val-fs01/Services/Methodes Production/0- IPR VALIDE</v>
+        <f>SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B3,"S:","/media/val-fs01/Services"),"\","/")," ","\ ")</f>
+        <v>/media/val-fs01/Services/Methodes\ Production/0-\ IPR\ VALIDE</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -467,8 +467,8 @@
         <v>4</v>
       </c>
       <c r="C4" s="2" t="str">
-        <f t="shared" ref="C4:C5" si="0">SUBSTITUTE(SUBSTITUTE(B4,"S:","\\val-fs01\Services"),"\","/")</f>
-        <v>//val-fs01/Services/Methodes Production/1- IPR AUTORISEES</v>
+        <f t="shared" ref="C4:C5" si="0">SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B4,"S:","/media/val-fs01/Services"),"\","/")," ","\ ")</f>
+        <v>/media/val-fs01/Services/Methodes\ Production/1-\ IPR\ AUTORISEES</v>
       </c>
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
@@ -482,7 +482,7 @@
       </c>
       <c r="C5" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>//val-fs01/Services/Methodes Production/IPR CARTE CMS/FICHE D'INSTRUCTION</v>
+        <v>/media/val-fs01/Services/Methodes\ Production/IPR\ CARTE\ CMS/FICHE\ D'INSTRUCTION</v>
       </c>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>

</xml_diff>